<commit_message>
Lógica de Devolução finalizada. Inicar processo de Substituição
</commit_message>
<xml_diff>
--- a/Termo de Responsabilidade Equipamentos de Medição.xlsx
+++ b/Termo de Responsabilidade Equipamentos de Medição.xlsx
@@ -70,9 +70,6 @@
     <t>Faixa Nominal</t>
   </si>
   <si>
-    <t>Motivo Devol.</t>
-  </si>
-  <si>
     <t>Data devol.</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>Data: ___/___/_____</t>
+  </si>
+  <si>
+    <t>Motivo</t>
   </si>
 </sst>
 </file>
@@ -527,22 +527,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -599,25 +614,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,7 +897,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G2"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -910,166 +910,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="40" t="s">
+      <c r="A1" s="42"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="42" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="43"/>
+      <c r="I1" s="48"/>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="45"/>
+      <c r="K1" s="50"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="42" t="s">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="43"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="2">
         <v>45293</v>
       </c>
-      <c r="K2" s="46"/>
+      <c r="K2" s="51"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="26" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="42" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="43"/>
+      <c r="I3" s="48"/>
       <c r="J3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="46"/>
+      <c r="K3" s="51"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="44" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="31"/>
+      <c r="I4" s="36"/>
       <c r="J4" s="4">
         <v>45658</v>
       </c>
-      <c r="K4" s="47"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="58"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="58"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="50"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="55"/>
     </row>
     <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="53"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
@@ -1087,30 +1087,30 @@
     <row r="12" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
       <c r="J12" s="5"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="5"/>
       <c r="K13" s="10"/>
     </row>
@@ -1130,7 +1130,7 @@
     <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1159,41 +1159,41 @@
       <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="35" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="36"/>
+      <c r="F17" s="41"/>
       <c r="G17" s="19" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="56"/>
+      <c r="K17" s="60"/>
     </row>
     <row r="18" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="25"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="17"/>
       <c r="J18" s="23"/>
-      <c r="K18" s="25"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
@@ -1252,16 +1252,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="E17:F17"/>
@@ -1276,6 +1266,16 @@
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alinhando fluxo de calibração para envio dos itens respeitando a regra de negócio
</commit_message>
<xml_diff>
--- a/Termo de Responsabilidade Equipamentos de Medição.xlsx
+++ b/Termo de Responsabilidade Equipamentos de Medição.xlsx
@@ -486,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,39 +527,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,10 +581,46 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,7 +900,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -910,166 +913,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="45" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="47" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="48"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="50"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="47" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="48"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="2">
         <v>45293</v>
       </c>
-      <c r="K2" s="51"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="31" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="47" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="48"/>
+      <c r="I3" s="37"/>
       <c r="J3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="51"/>
+      <c r="K3" s="40"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="49" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="36"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="4">
         <v>45658</v>
       </c>
-      <c r="K4" s="52"/>
+      <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="39"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
       <c r="G6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="52"/>
     </row>
     <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="52"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="55"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
     </row>
     <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="56"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="58"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="56"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="58"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
     </row>
     <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
@@ -1087,30 +1090,30 @@
     <row r="12" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="5"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="5"/>
       <c r="K13" s="10"/>
     </row>
@@ -1159,15 +1162,15 @@
       <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="40" t="s">
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="41"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="19" t="s">
         <v>17</v>
       </c>
@@ -1177,23 +1180,23 @@
       <c r="I17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="59" t="s">
+      <c r="J17" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="60"/>
+      <c r="K17" s="50"/>
     </row>
     <row r="18" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="54"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+      <c r="H18" s="61"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="24"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="54"/>
     </row>
     <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
@@ -1252,6 +1255,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="E17:F17"/>
@@ -1268,14 +1279,6 @@
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>